<commit_message>
Finished design sheet to use a common design for all four regulators
</commit_message>
<xml_diff>
--- a/MultiSpork/documentation/regulator-design-sheet.xlsx
+++ b/MultiSpork/documentation/regulator-design-sheet.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="+10V regulator" sheetId="1" r:id="rId1"/>
-    <sheet name="-10V regulator" sheetId="2" r:id="rId2"/>
+    <sheet name="+10V regulator (LT3580)" sheetId="1" r:id="rId1"/>
+    <sheet name="+5V regulator" sheetId="3" r:id="rId2"/>
+    <sheet name="-10V regulator" sheetId="2" r:id="rId3"/>
+    <sheet name="+10V regulator" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="56">
   <si>
     <t>V</t>
   </si>
@@ -220,6 +222,18 @@
     <t>Minimum battery voltage, after diode</t>
   </si>
   <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Maximum current</t>
+  </si>
+  <si>
+    <t>µH</t>
+  </si>
+  <si>
+    <t>Value to prevent subharmonics</t>
+  </si>
+  <si>
     <r>
       <t>I</t>
     </r>
@@ -232,14 +246,257 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>out(max)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L-peak</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max(USB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max(bat)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min(bat)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min(USB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>final</t>
+    </r>
+  </si>
+  <si>
+    <t>Selected value</t>
+  </si>
+  <si>
+    <t>µF</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>out</t>
     </r>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Maximum current</t>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>series</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parallel</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>series</t>
+    </r>
+  </si>
+  <si>
+    <t>pF</t>
+  </si>
+  <si>
+    <t>nF</t>
+  </si>
+  <si>
+    <t>Note that these are taken from the SEPIC converter in datasheet rather than calculated. They'll be done properly later.</t>
+  </si>
+  <si>
+    <r>
+      <t>|V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>out</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L1-peak</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L2-peak</t>
+    </r>
   </si>
   <si>
     <r>
@@ -254,14 +511,116 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>min</t>
-    </r>
-  </si>
-  <si>
-    <t>µH</t>
-  </si>
-  <si>
-    <t>Value to prevent subharmonics</t>
+      <t>1-final</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2-final</t>
+    </r>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>LT3580</t>
+  </si>
+  <si>
+    <t>AD1614</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1fb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2fb</t>
+    </r>
+  </si>
+  <si>
+    <t>µs</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on(bat)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>on(USB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ripple(max)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -311,11 +670,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,6 +970,15 @@
     <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
@@ -623,16 +995,16 @@
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.35</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -640,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -680,8 +1052,8 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <f>($B$2-$B$4+0.7)/($B$2+0.7+0.3)</f>
-        <v>0.79090909090909089</v>
+        <f>($B$2-$B$4+0.7)/($B$2+0.7-0.3)</f>
+        <v>0.78846153846153855</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -692,8 +1064,8 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <f>($B$2-$B$5+0.7)/($B$2+0.7+0.3)</f>
-        <v>0.51818181818181819</v>
+        <f>($B$2-$B$5+0.7)/($B$2+0.7-0.3)</f>
+        <v>0.54807692307692313</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -705,7 +1077,7 @@
       </c>
       <c r="B9">
         <f>91.9/(B10+1)</f>
-        <v>2.9645161290322584</v>
+        <v>1.9145833333333335</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -716,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>3</v>
@@ -728,7 +1100,7 @@
       </c>
       <c r="B11" s="2">
         <f>(1/B9)*1000</f>
-        <v>337.32317736670291</v>
+        <v>522.30685527747539</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>13</v>
@@ -743,7 +1115,7 @@
       </c>
       <c r="B12" s="2">
         <f>(B11-60)/B11</f>
-        <v>0.82212903225806455</v>
+        <v>0.88512499999999994</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -751,32 +1123,173 @@
     </row>
     <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <f>B7*B5/(2*B9*(2.4-(B2*B3/(B2*0.88))))</f>
-        <v>0.52782583508818615</v>
+        <v>29</v>
+      </c>
+      <c r="B13" s="2">
+        <f>$B$7*$B$4/(2*$B$9*(2.4-($B$2*$B$3/($B$4*0.88))))</f>
+        <v>0.63623701309999303</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2">
+        <f>$B$8*$B$5/(2*$B$9*(2.4-($B$2*$B$3/($B$5*0.88))))</f>
+        <v>0.44602091721913434</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="2">
+        <f>$B$4*(2*$B$7-1)/((1-$B$7)*$B$9)</f>
+        <v>3.5611831041646078</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="B14">
-        <f>B5*(2*B7-1)/((1-B7)*B9)</f>
-        <v>4.6931920329280397</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2">
+        <f>$B$5*(2*$B$8-1)/((1-$B$8)*$B$9)</f>
+        <v>0.55564559072071928</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2">
+        <f>((B5-0.3)/0.095)*(B8/B9)</f>
+        <v>14.162551268100779</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2">
+        <f>((B4-0.3)/0.095)*(B7/B9)</f>
+        <v>9.5368579647830547</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>26</v>
       </c>
+      <c r="B20" s="2">
+        <f>((B2*B3)/(B4*0.88))+((B4*B7)/(2*B19*B9))</f>
+        <v>1.6767046881301506</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21">
+        <v>4.7</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="2">
+        <v>22</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -784,18 +1297,859 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>-10</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <f>((B2-1.215)/0.0000833)/1000</f>
+        <v>45.43817527010804</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <f>($B$2-$B$4+0.7)/($B$2+0.7-0.3)</f>
+        <v>0.59259259259259256</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>91.9/(B8+1)</f>
+        <v>1.9145833333333335</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <f>(1/B7)*1000</f>
+        <v>522.30685527747539</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <f>(B9-60)/B9</f>
+        <v>0.88512499999999994</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2">
+        <f>$B$6*$B$4/(2*$B$7*(2.4-($B$2*$B$3/($B$4*0.88))))</f>
+        <v>1.0912393937421141</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2">
+        <f>$B$4*(2*$B$6-1)/((1-$B$6)*$B$7)</f>
+        <v>0.59353051736076734</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2">
+        <f>((B4-0.3)/0.095)*(B6/B7)</f>
+        <v>7.1677198073166215</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2">
+        <f>((B2*B3)/(B4*0.88))+((B4*B6)/(2*B14*B7))</f>
+        <v>2.1099368732665793</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>4.7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="2">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D18:D20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <f>((B2+0.005)/0.0000833)/1000</f>
+        <v>120.10804321728692</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <f>($B$2+0.7)/($B$2+$B$4+0.7-0.3)</f>
+        <v>0.8294573643410853</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <f>91.9/(B8+1)</f>
+        <v>1.9145833333333335</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <f>(1/B7)*1000</f>
+        <v>522.30685527747539</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <f>(B9-60)/B9</f>
+        <v>0.88512499999999994</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2">
+        <f>$B$6*$B$4/(2*$B$7*(2.4-($B$2*$B$3/($B$4*0.75))-$B$3))</f>
+        <v>2.9538495515163796</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2">
+        <f>$B$4*(2*$B$6-1)/((1-$B$6)*$B$7)</f>
+        <v>5.0450093975665258</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2">
+        <f>((B4-0.3)/0.095)*(B6/B7)</f>
+        <v>10.0327240907644</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2">
+        <f>((B2*B3)/(B4*0.75))+((B4*B6)/(2*B14*B7))</f>
+        <v>1.9569231807407783</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="2">
+        <f>B3+((B2*(1-B6))/(2*B15*B7))</f>
+        <v>0.42422965643478328</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>4.7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="36.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>0.35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>2.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3">
+        <f>B7*((B2-1.245)/1.245)</f>
+        <v>70.321285140562239</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f>($B$2-$B$4)/$B$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <f>($B$2-$B$5)/$B$2</f>
+        <v>0.5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1.3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2">
+        <f>B8/B10</f>
+        <v>0.57692307692307687</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2">
+        <f>B9/B10</f>
+        <v>0.38461538461538458</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <f>B4*B11/$B$13</f>
+        <v>3.6057692307692299</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2">
+        <f>B5*B12/$B$13</f>
+        <v>4.8076923076923066</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2">
+        <f>(B3*(B2/B4))+(B13/2)</f>
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19">
+        <v>22</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="2">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D20:D22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated regulator design sheet to use smaller inductors
</commit_message>
<xml_diff>
--- a/MultiSpork/documentation/regulator-design-sheet.xlsx
+++ b/MultiSpork/documentation/regulator-design-sheet.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="+10V regulator (LT3580)" sheetId="1" r:id="rId1"/>
-    <sheet name="+5V regulator" sheetId="3" r:id="rId2"/>
-    <sheet name="-10V regulator" sheetId="2" r:id="rId3"/>
-    <sheet name="+10V regulator" sheetId="4" r:id="rId4"/>
+    <sheet name="3.3V SEPIC regulator" sheetId="5" r:id="rId2"/>
+    <sheet name="+5V SEPIC regulator" sheetId="3" r:id="rId3"/>
+    <sheet name="-10V regulator" sheetId="2" r:id="rId4"/>
+    <sheet name="+10V regulator" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="76">
   <si>
     <t>V</t>
   </si>
@@ -621,6 +622,249 @@
       </rPr>
       <t>ripple(max)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>d</t>
+    </r>
+  </si>
+  <si>
+    <t>Diode voltage drop</t>
+  </si>
+  <si>
+    <t>2323 (5858 metric)</t>
+  </si>
+  <si>
+    <t>SRR5018-3R9Y</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L1-peak(bat)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L2-peak(bat)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L1-peak(USB)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L2-peak(USB)</t>
+    </r>
+  </si>
+  <si>
+    <t>L p/n</t>
+  </si>
+  <si>
+    <t>L package</t>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> p/n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> package</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> p/n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>L</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> package</t>
+    </r>
+  </si>
+  <si>
+    <t>1008 (2520 metric)</t>
+  </si>
+  <si>
+    <t>252012CDMCDS-2R2MC</t>
+  </si>
+  <si>
+    <t>SRR5028-5R3Y</t>
+  </si>
+  <si>
+    <t>PM1008S-5R6M-RC</t>
   </si>
 </sst>
 </file>
@@ -670,7 +914,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -679,6 +923,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,14 +1206,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -974,10 +1222,10 @@
       <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1204,7 +1452,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="2">
-        <v>6</v>
+        <v>3.9</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
@@ -1219,7 +1467,7 @@
       </c>
       <c r="B20" s="2">
         <f>((B2*B3)/(B4*0.88))+((B4*B7)/(2*B19*B9))</f>
-        <v>1.6767046881301506</v>
+        <v>1.7229023174030287</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>21</v>
@@ -1285,10 +1533,32 @@
       </c>
       <c r="D25" s="5"/>
     </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1297,32 +1567,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="35.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>3.3</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -1333,247 +1606,876 @@
     </row>
     <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B3">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B4">
-        <v>2.5</v>
+        <v>0.8</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B7" s="3">
+        <f>((B2-1.215)/0.0000833)/1000</f>
+        <v>25.030012004801918</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <f>($B$2+$B$3)/($B$5+$B$2+$B$3-0.3)</f>
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <f>($B$2+$B$3)/($B$6+$B$2+$B$3-0.3)</f>
+        <v>0.45977011494252878</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f>91.9/(B11+1)</f>
+        <v>1.9145833333333335</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <f>(1/B10)*1000</f>
+        <v>522.30685527747539</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2">
+        <f>(B12-60)/B12</f>
+        <v>0.88512499999999994</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="2">
+        <f>$B$8*$B$5/(2*$B$10*(2.4-($B$2*$B$4/($B$5*0.75))-$B$4))</f>
+        <v>2.1938291972340229</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2">
+        <f>$B$8*$B$6/(2*$B$10*(2.4-($B$2*$B$4/($B$6*0.75))-$B$4))</f>
+        <v>0.94021251310029452</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2">
+        <f>$B$5*(2*$B$8-1)/((1-$B$8)*$B$10)</f>
+        <v>1.0683549312493814</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2">
+        <f>$B$6*(2*$B$9-1)/((1-$B$9)*$B$10)</f>
+        <v>-0.38895191350450259</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2">
+        <f>((B6-0.3)/0.095)*(B9/B10)</f>
+        <v>11.880664100685468</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <f>((B5-0.3)/0.095)*(B8/B10)</f>
+        <v>7.8035659192560001</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="2">
+        <f>(($B$2*$B$4)/($B$5*0.75))+(($B$5*$B$8)/(2*$B$20*$B$10))</f>
+        <v>1.5994614572131509</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2">
+        <f>$B$4+(($B$2*(1-$B$8))/(2*$B$21*$B$10))</f>
+        <v>0.93900101793674751</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2">
+        <f>(($B$2*$B$4)/($B$5*0.75))+(($B$6*$B$9)/(2*$B$20*$B$10))</f>
+        <v>1.6808875941888588</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="4" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="2">
+        <f>$B$4+(($B$2*(1-$B$9))/(2*$B$21*$B$10))</f>
+        <v>1.0116243292934599</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>4.7</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="2">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="2">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:C35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
         <f>((B2-1.215)/0.0000833)/1000</f>
         <v>45.43817527010804</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <f>($B$2-$B$4+0.7)/($B$2+0.7-0.3)</f>
-        <v>0.59259259259259256</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B8" s="2">
+        <f>($B$2+$B$3)/($B$5+$B$2+$B$3-0.3)</f>
+        <v>0.72151898734177222</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <f>($B$2+$B$3)/($B$6+$B$2+$B$3-0.3)</f>
+        <v>0.54807692307692313</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <f>91.9/(B8+1)</f>
+      <c r="B10" s="4">
+        <f>91.9/(B11+1)</f>
         <v>1.9145833333333335</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="2">
         <v>47</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
-        <f>(1/B7)*1000</f>
+      <c r="B12" s="2">
+        <f>(1/B10)*1000</f>
         <v>522.30685527747539</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
-        <f>(B9-60)/B9</f>
+      <c r="B13" s="2">
+        <f>(B12-60)/B12</f>
         <v>0.88512499999999994</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="2">
-        <f>$B$6*$B$4/(2*$B$7*(2.4-($B$2*$B$3/($B$4*0.88))))</f>
-        <v>1.0912393937421141</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="2">
-        <f>$B$4*(2*$B$6-1)/((1-$B$6)*$B$7)</f>
-        <v>0.59353051736076734</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2">
-        <f>((B4-0.3)/0.095)*(B6/B7)</f>
-        <v>7.1677198073166215</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>31</v>
-      </c>
       <c r="B14" s="2">
-        <v>6</v>
+        <f>$B$8*$B$5/(2*$B$10*(2.4-($B$2*$B$4/($B$5*0.75))-$B$4))</f>
+        <v>0.50471559817161127</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2">
+        <f>$B$8*$B$6/(2*$B$10*(2.4-($B$2*$B$4/($B$6*0.75))-$B$4))</f>
+        <v>0.64236530676386872</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2">
+        <f>$B$5*(2*$B$8-1)/((1-$B$8)*$B$10)</f>
+        <v>2.0773568107626876</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2">
+        <f>$B$6*(2*$B$9-1)/((1-$B$9)*$B$10)</f>
+        <v>0.55564559072071928</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="2">
+        <f>((B6-0.3)/0.095)*(B9/B10)</f>
+        <v>14.162551268100779</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2">
+        <f>((B5-0.3)/0.095)*(B8/B10)</f>
+        <v>8.7271525185603505</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <f>((B2*B3)/(B4*0.88))+((B4*B6)/(2*B14*B7))</f>
-        <v>2.1099368732665793</v>
-      </c>
-      <c r="C15" s="1" t="s">
+    <row r="21" spans="1:4" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="2">
+        <f>(($B$2*$B$4)/($B$5*0.75))+(($B$5*$B$8)/(2*$B$20*$B$10))</f>
+        <v>1.2807884355879562</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="2">
+        <f>$B$4+(($B$2*(1-$B$8))/(2*$B$21*$B$10))</f>
+        <v>0.5652869795181884</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="2">
+        <f>(($B$2*$B$4)/($B$5*0.75))+(($B$6*$B$9)/(2*$B$20*$B$10))</f>
+        <v>1.3919670463740106</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="2">
+        <f>$B$4+(($B$2*(1-$B$9))/(2*$B$21*$B$10))</f>
+        <v>0.66823013765342376</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
+      <c r="B26" s="4">
         <v>4.7</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
+      <c r="B27" s="4">
         <v>20</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B28" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B29" s="2">
         <v>22</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B30" s="2">
         <v>10</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D30" s="5"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A32" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A33" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="6"/>
+    </row>
+    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A35" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="D28:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,10 +2488,10 @@
       <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1751,7 +2653,7 @@
         <v>45</v>
       </c>
       <c r="B14" s="2">
-        <v>6</v>
+        <v>5.3</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -1765,7 +2667,7 @@
         <v>46</v>
       </c>
       <c r="B15" s="2">
-        <v>6</v>
+        <v>5.6</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>23</v>
@@ -1777,7 +2679,7 @@
       </c>
       <c r="B16" s="2">
         <f>((B2*B3)/(B4*0.75))+((B4*B6)/(2*B14*B7))</f>
-        <v>1.9569231807407783</v>
+        <v>1.968843852410944</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>21</v>
@@ -1789,7 +2691,7 @@
       </c>
       <c r="B17" s="2">
         <f>B3+((B2*(1-B6))/(2*B15*B7))</f>
-        <v>0.42422965643478328</v>
+        <v>0.42953177475155352</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>21</v>
@@ -1855,16 +2757,60 @@
       </c>
       <c r="D22" s="5"/>
     </row>
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A24" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="B27:C27"/>
     <mergeCell ref="D20:D22"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -1881,10 +2827,10 @@
       <c r="A1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="4"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">

</xml_diff>